<commit_message>
chore: preencher células vazias
Identificar e preencher com 0,0 todas as células que acidentalmente ficaram vazias na planilha.
</commit_message>
<xml_diff>
--- a/Base de Dados/Dados Tratados/OUTUBRO_2022.xlsx
+++ b/Base de Dados/Dados Tratados/OUTUBRO_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\GitHub\Projeto-Painel-de-BI-Dados-Agricolas\Base de Dados\Dados Tratados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED698F7-DD5E-4610-9067-11DC58D4A71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E904DD-C948-4497-83DE-C5C0BD28A3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AREA_POR_PRODUTO" sheetId="1" r:id="rId1"/>
@@ -362,10 +362,85 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -476,78 +551,6 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -653,10 +656,7 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -956,44 +956,44 @@
   <autoFilter ref="A1:AM25" xr:uid="{5B7D321A-43AE-4A82-BD55-3D36C41B7E32}"/>
   <tableColumns count="39">
     <tableColumn id="1" xr3:uid="{8CF1AF50-3446-4E75-8105-3A27A31DC53D}" name="PRODUTO"/>
-    <tableColumn id="2" xr3:uid="{B84906ED-0B3E-4BAF-823C-613564EC7F44}" name="NORTE" dataDxfId="120"/>
-    <tableColumn id="3" xr3:uid="{84B9811A-583F-4CE3-B96E-FD8D3F9C0AF7}" name="RR" dataDxfId="119"/>
-    <tableColumn id="4" xr3:uid="{0AFF1D5D-3E87-4339-BBA1-770DC84997E0}" name="RO" dataDxfId="118"/>
-    <tableColumn id="5" xr3:uid="{8E7E000F-2618-4C1D-A0A3-786BAD1CCA1E}" name="AC" dataDxfId="117"/>
-    <tableColumn id="6" xr3:uid="{8FDC185D-309C-44F0-909D-47D36E4E88C7}" name="AM" dataDxfId="116"/>
-    <tableColumn id="7" xr3:uid="{FCFBA294-1B56-4D43-81BD-8397D063FB54}" name="AP" dataDxfId="115"/>
-    <tableColumn id="8" xr3:uid="{A4D89CF5-1E5F-4A95-9E6F-6AF87D6DC899}" name="PA" dataDxfId="114"/>
-    <tableColumn id="9" xr3:uid="{CBEB4E66-65D5-43C3-A560-E78883927AF4}" name="TO" dataDxfId="113"/>
-    <tableColumn id="10" xr3:uid="{E7D25C84-64C7-44D2-85A6-1289EF929C61}" name="NORDESTE" dataDxfId="112"/>
-    <tableColumn id="11" xr3:uid="{3A9FA498-3724-4EB1-92DC-966AAB9D214D}" name="MA" dataDxfId="111"/>
-    <tableColumn id="12" xr3:uid="{217BE2AA-49BC-4EFB-A2E9-A68DAFEE98F1}" name="PI" dataDxfId="110"/>
-    <tableColumn id="13" xr3:uid="{2A2F8CD6-E44E-48F7-95FF-898DA8413AFD}" name="CE" dataDxfId="109"/>
-    <tableColumn id="14" xr3:uid="{A6E9090C-1AB9-4D6E-9F99-ABDA730D9CA6}" name="RN" dataDxfId="108"/>
-    <tableColumn id="15" xr3:uid="{C74DAA05-C155-4F4D-B631-EB31FBB3665F}" name="PB" dataDxfId="107"/>
-    <tableColumn id="16" xr3:uid="{E5A10D15-FEE8-4661-ADBA-FB28CEA9267C}" name="PE" dataDxfId="106"/>
-    <tableColumn id="17" xr3:uid="{D1DA04F7-F9F0-4017-AE33-C5C1E7CE5AC0}" name="AL" dataDxfId="105"/>
-    <tableColumn id="18" xr3:uid="{DD2B9F5D-C570-466E-82CC-C54D2042ADFD}" name="SE" dataDxfId="104"/>
-    <tableColumn id="19" xr3:uid="{A2536CAA-3E99-4275-8AFB-0F230AD1FE08}" name="BA" dataDxfId="103"/>
-    <tableColumn id="20" xr3:uid="{C9DE622E-9653-49C4-97A9-6F44C0598F06}" name="CENTRO-OESTE" dataDxfId="102"/>
-    <tableColumn id="21" xr3:uid="{625EA772-B512-443B-A734-AF5CE77AB668}" name="MT" dataDxfId="101"/>
-    <tableColumn id="22" xr3:uid="{71A57575-7815-481F-AAAC-8C1EE9703912}" name="MS" dataDxfId="100"/>
-    <tableColumn id="23" xr3:uid="{F0365580-4820-46C6-A7D7-BD7C897237CB}" name="GO" dataDxfId="99"/>
-    <tableColumn id="24" xr3:uid="{A5D6C791-8D94-4B52-8C0C-39F7AD4AC4E1}" name="DF" dataDxfId="98"/>
-    <tableColumn id="25" xr3:uid="{3C464D88-F9B1-4C7A-8784-1840561093C3}" name="SUDESTE" dataDxfId="97"/>
-    <tableColumn id="26" xr3:uid="{1184085B-389F-4DFA-BAAA-79A73F5D58E9}" name="MG" dataDxfId="96"/>
-    <tableColumn id="27" xr3:uid="{1FD7AAC9-8B22-4599-8C41-97B306E682A8}" name="ES" dataDxfId="95"/>
-    <tableColumn id="28" xr3:uid="{3789E530-8644-46B9-A1D9-538F173953B6}" name="RJ" dataDxfId="94"/>
-    <tableColumn id="29" xr3:uid="{4B510379-3A08-42EB-8F76-653D7A9A0F0C}" name="SP" dataDxfId="93"/>
-    <tableColumn id="30" xr3:uid="{B7137113-AFD6-4F75-AE3E-0C0A27D770EB}" name="SUL" dataDxfId="92"/>
-    <tableColumn id="31" xr3:uid="{725B070C-B20E-4909-860C-25B32C284E06}" name="PR" dataDxfId="91"/>
-    <tableColumn id="32" xr3:uid="{4407D65F-AE79-48AC-9A84-33DCE4A2ADA4}" name="SC" dataDxfId="90"/>
-    <tableColumn id="33" xr3:uid="{88C455AC-C842-489F-84B2-E60D576F9F16}" name="RS" dataDxfId="89"/>
-    <tableColumn id="34" xr3:uid="{F04DD72A-4B16-4880-860B-5C4A2F256C93}" name="NORTE-NORDESTE" dataDxfId="88"/>
-    <tableColumn id="35" xr3:uid="{83D2B4A6-D70A-4652-89BB-1ED9B337F34A}" name="CENTRO-SUL" dataDxfId="87"/>
-    <tableColumn id="36" xr3:uid="{E90095A4-CB96-450E-A159-B808E8913751}" name="BRASIL" dataDxfId="85"/>
-    <tableColumn id="37" xr3:uid="{5796B11A-3AF2-4B43-92FF-178971C3DBD9}" name="ANO" dataDxfId="86"/>
-    <tableColumn id="38" xr3:uid="{5B4B4C2C-6AED-479F-B62E-92551DACC89D}" name="MÊS" dataDxfId="122"/>
-    <tableColumn id="39" xr3:uid="{453C9B87-B335-49FF-BF33-6444C74EE93B}" name="SAFRA" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{B84906ED-0B3E-4BAF-823C-613564EC7F44}" name="NORTE" dataDxfId="122"/>
+    <tableColumn id="3" xr3:uid="{84B9811A-583F-4CE3-B96E-FD8D3F9C0AF7}" name="RR" dataDxfId="121"/>
+    <tableColumn id="4" xr3:uid="{0AFF1D5D-3E87-4339-BBA1-770DC84997E0}" name="RO" dataDxfId="120"/>
+    <tableColumn id="5" xr3:uid="{8E7E000F-2618-4C1D-A0A3-786BAD1CCA1E}" name="AC" dataDxfId="119"/>
+    <tableColumn id="6" xr3:uid="{8FDC185D-309C-44F0-909D-47D36E4E88C7}" name="AM" dataDxfId="118"/>
+    <tableColumn id="7" xr3:uid="{FCFBA294-1B56-4D43-81BD-8397D063FB54}" name="AP" dataDxfId="117"/>
+    <tableColumn id="8" xr3:uid="{A4D89CF5-1E5F-4A95-9E6F-6AF87D6DC899}" name="PA" dataDxfId="116"/>
+    <tableColumn id="9" xr3:uid="{CBEB4E66-65D5-43C3-A560-E78883927AF4}" name="TO" dataDxfId="115"/>
+    <tableColumn id="10" xr3:uid="{E7D25C84-64C7-44D2-85A6-1289EF929C61}" name="NORDESTE" dataDxfId="114"/>
+    <tableColumn id="11" xr3:uid="{3A9FA498-3724-4EB1-92DC-966AAB9D214D}" name="MA" dataDxfId="113"/>
+    <tableColumn id="12" xr3:uid="{217BE2AA-49BC-4EFB-A2E9-A68DAFEE98F1}" name="PI" dataDxfId="112"/>
+    <tableColumn id="13" xr3:uid="{2A2F8CD6-E44E-48F7-95FF-898DA8413AFD}" name="CE" dataDxfId="111"/>
+    <tableColumn id="14" xr3:uid="{A6E9090C-1AB9-4D6E-9F99-ABDA730D9CA6}" name="RN" dataDxfId="110"/>
+    <tableColumn id="15" xr3:uid="{C74DAA05-C155-4F4D-B631-EB31FBB3665F}" name="PB" dataDxfId="109"/>
+    <tableColumn id="16" xr3:uid="{E5A10D15-FEE8-4661-ADBA-FB28CEA9267C}" name="PE" dataDxfId="108"/>
+    <tableColumn id="17" xr3:uid="{D1DA04F7-F9F0-4017-AE33-C5C1E7CE5AC0}" name="AL" dataDxfId="107"/>
+    <tableColumn id="18" xr3:uid="{DD2B9F5D-C570-466E-82CC-C54D2042ADFD}" name="SE" dataDxfId="106"/>
+    <tableColumn id="19" xr3:uid="{A2536CAA-3E99-4275-8AFB-0F230AD1FE08}" name="BA" dataDxfId="105"/>
+    <tableColumn id="20" xr3:uid="{C9DE622E-9653-49C4-97A9-6F44C0598F06}" name="CENTRO-OESTE" dataDxfId="104"/>
+    <tableColumn id="21" xr3:uid="{625EA772-B512-443B-A734-AF5CE77AB668}" name="MT" dataDxfId="103"/>
+    <tableColumn id="22" xr3:uid="{71A57575-7815-481F-AAAC-8C1EE9703912}" name="MS" dataDxfId="102"/>
+    <tableColumn id="23" xr3:uid="{F0365580-4820-46C6-A7D7-BD7C897237CB}" name="GO" dataDxfId="101"/>
+    <tableColumn id="24" xr3:uid="{A5D6C791-8D94-4B52-8C0C-39F7AD4AC4E1}" name="DF" dataDxfId="100"/>
+    <tableColumn id="25" xr3:uid="{3C464D88-F9B1-4C7A-8784-1840561093C3}" name="SUDESTE" dataDxfId="99"/>
+    <tableColumn id="26" xr3:uid="{1184085B-389F-4DFA-BAAA-79A73F5D58E9}" name="MG" dataDxfId="98"/>
+    <tableColumn id="27" xr3:uid="{1FD7AAC9-8B22-4599-8C41-97B306E682A8}" name="ES" dataDxfId="97"/>
+    <tableColumn id="28" xr3:uid="{3789E530-8644-46B9-A1D9-538F173953B6}" name="RJ" dataDxfId="96"/>
+    <tableColumn id="29" xr3:uid="{4B510379-3A08-42EB-8F76-653D7A9A0F0C}" name="SP" dataDxfId="95"/>
+    <tableColumn id="30" xr3:uid="{B7137113-AFD6-4F75-AE3E-0C0A27D770EB}" name="SUL" dataDxfId="94"/>
+    <tableColumn id="31" xr3:uid="{725B070C-B20E-4909-860C-25B32C284E06}" name="PR" dataDxfId="93"/>
+    <tableColumn id="32" xr3:uid="{4407D65F-AE79-48AC-9A84-33DCE4A2ADA4}" name="SC" dataDxfId="92"/>
+    <tableColumn id="33" xr3:uid="{88C455AC-C842-489F-84B2-E60D576F9F16}" name="RS" dataDxfId="91"/>
+    <tableColumn id="34" xr3:uid="{F04DD72A-4B16-4880-860B-5C4A2F256C93}" name="NORTE-NORDESTE" dataDxfId="90"/>
+    <tableColumn id="35" xr3:uid="{83D2B4A6-D70A-4652-89BB-1ED9B337F34A}" name="CENTRO-SUL" dataDxfId="89"/>
+    <tableColumn id="36" xr3:uid="{E90095A4-CB96-450E-A159-B808E8913751}" name="BRASIL" dataDxfId="88"/>
+    <tableColumn id="37" xr3:uid="{5796B11A-3AF2-4B43-92FF-178971C3DBD9}" name="ANO" dataDxfId="87"/>
+    <tableColumn id="38" xr3:uid="{5B4B4C2C-6AED-479F-B62E-92551DACC89D}" name="MÊS" dataDxfId="86"/>
+    <tableColumn id="39" xr3:uid="{453C9B87-B335-49FF-BF33-6444C74EE93B}" name="SAFRA" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1041,44 +1041,44 @@
   <autoFilter ref="A1:AM25" xr:uid="{F205EC7A-49EF-4699-9240-6A619C4E0678}"/>
   <tableColumns count="39">
     <tableColumn id="1" xr3:uid="{6051C5E2-E2B7-4BEB-BC76-2DCAA50A7C15}" name="PRODUTO"/>
-    <tableColumn id="2" xr3:uid="{B8D0D550-3F4A-455D-B730-DC7BB52A9B2A}" name="NORTE" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{F0C3B647-0AA7-4BDE-9C13-1E481DDA789C}" name="RR" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{2118BB87-FCC8-403D-8FCA-D68B9ED42B8C}" name="RO" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{3CA4EDC5-768A-430C-8DF0-0D22D3452853}" name="AC" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{7362E812-6294-4692-A499-A02354A455C2}" name="AM" dataDxfId="55"/>
-    <tableColumn id="7" xr3:uid="{482DE189-3576-4B8E-BF1A-9C58B5F5C6ED}" name="AP" dataDxfId="54"/>
-    <tableColumn id="8" xr3:uid="{0E0FA7BD-E6EA-426B-B8B1-9665A67EE819}" name="PA" dataDxfId="53"/>
-    <tableColumn id="9" xr3:uid="{9ABF8262-0C59-4BAA-8D66-6D70743CECED}" name="TO" dataDxfId="52"/>
-    <tableColumn id="10" xr3:uid="{96D8ACAF-FFFE-4005-ADC1-94AA97CD6038}" name="NORDESTE" dataDxfId="51"/>
-    <tableColumn id="11" xr3:uid="{1FABF4C2-AC99-4575-B4A2-682FB02C27AB}" name="MA" dataDxfId="50"/>
-    <tableColumn id="12" xr3:uid="{6E7000A1-CF81-4A5C-AF79-B5A606493E58}" name="PI" dataDxfId="49"/>
-    <tableColumn id="13" xr3:uid="{5804C6F2-0132-4A60-8701-6454E76B39E1}" name="CE" dataDxfId="48"/>
-    <tableColumn id="14" xr3:uid="{FAC246D4-9925-4737-BA6E-C12890CC3492}" name="RN" dataDxfId="47"/>
-    <tableColumn id="15" xr3:uid="{70365A79-11D8-4822-868C-B390282D31AA}" name="PB" dataDxfId="46"/>
-    <tableColumn id="16" xr3:uid="{C5EA46D4-2A74-4A1B-8628-EDE27732EBC1}" name="PE" dataDxfId="45"/>
-    <tableColumn id="17" xr3:uid="{3AB16384-A9C1-4EAE-B1D3-B6980668DDFB}" name="AL" dataDxfId="44"/>
-    <tableColumn id="18" xr3:uid="{5550B480-640D-47F3-98E2-47360C39B350}" name="SE" dataDxfId="43"/>
-    <tableColumn id="19" xr3:uid="{AC7410A2-BEC3-4F36-9DE3-007ABEDAFE77}" name="BA" dataDxfId="42"/>
-    <tableColumn id="20" xr3:uid="{EF9CC834-4DE2-4F12-A01F-E188C35BB745}" name="CENTRO-OESTE" dataDxfId="41"/>
-    <tableColumn id="21" xr3:uid="{43361983-B660-4F10-8172-158B7FE088A3}" name="MT" dataDxfId="40"/>
-    <tableColumn id="22" xr3:uid="{1D87111A-4709-4B48-BC75-F06DA78D87CB}" name="MS" dataDxfId="39"/>
-    <tableColumn id="23" xr3:uid="{8C8B08DD-2483-4E25-AB6C-69DC01B3EB3D}" name="GO" dataDxfId="38"/>
-    <tableColumn id="24" xr3:uid="{9D3A4E55-E1CC-4509-9BBA-1BA1B5720931}" name="DF" dataDxfId="37"/>
-    <tableColumn id="25" xr3:uid="{64CEA2A0-9627-43CF-9192-24F44872CC96}" name="SUDESTE" dataDxfId="36"/>
-    <tableColumn id="26" xr3:uid="{4FBE3EC3-154E-4DF3-ABB6-B6DEFFC26271}" name="MG" dataDxfId="35"/>
-    <tableColumn id="27" xr3:uid="{B6B47D99-4133-4D01-BF64-2BBBE6D3BE49}" name="ES" dataDxfId="34"/>
-    <tableColumn id="28" xr3:uid="{7CC112A7-D0E8-4317-B401-EC4CD011155C}" name="RJ" dataDxfId="33"/>
-    <tableColumn id="29" xr3:uid="{14E6FF96-46F0-467D-A5A3-F1C831072AA9}" name="SP" dataDxfId="32"/>
-    <tableColumn id="30" xr3:uid="{932BDB91-3454-40CD-B097-52A8AA0A2F81}" name="SUL" dataDxfId="31"/>
-    <tableColumn id="31" xr3:uid="{AA858ED8-15B1-4985-9F57-E0EE2783C677}" name="PR" dataDxfId="30"/>
-    <tableColumn id="32" xr3:uid="{D302D227-008B-444D-87CF-C19499331330}" name="SC" dataDxfId="29"/>
-    <tableColumn id="33" xr3:uid="{65AB5642-25AB-4920-8029-D56BC42AB123}" name="RS" dataDxfId="28"/>
-    <tableColumn id="34" xr3:uid="{7666B84C-5946-494A-83CA-2B24D2CF0DC8}" name="NORTE-NORDESTE" dataDxfId="27"/>
-    <tableColumn id="35" xr3:uid="{633B8894-AE4A-45AC-B1C9-B4EAA702D9F9}" name="CENTRO-SUL" dataDxfId="26"/>
-    <tableColumn id="36" xr3:uid="{6BB08E62-BEF0-4192-83F6-2E12E9E586B8}" name="BRASIL" dataDxfId="24"/>
-    <tableColumn id="37" xr3:uid="{ECC44396-0C86-4DF0-B859-53097AD13988}" name="ANO" dataDxfId="25"/>
-    <tableColumn id="38" xr3:uid="{57AEF2DA-BFBE-4B5B-ABC0-477C4D3CA382}" name="MÊS" dataDxfId="61"/>
-    <tableColumn id="39" xr3:uid="{4AF1745A-E1C0-4A75-AFC1-E75F141DCCAA}" name="SAFRA" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{B8D0D550-3F4A-455D-B730-DC7BB52A9B2A}" name="NORTE" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{F0C3B647-0AA7-4BDE-9C13-1E481DDA789C}" name="RR" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{2118BB87-FCC8-403D-8FCA-D68B9ED42B8C}" name="RO" dataDxfId="59"/>
+    <tableColumn id="5" xr3:uid="{3CA4EDC5-768A-430C-8DF0-0D22D3452853}" name="AC" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{7362E812-6294-4692-A499-A02354A455C2}" name="AM" dataDxfId="57"/>
+    <tableColumn id="7" xr3:uid="{482DE189-3576-4B8E-BF1A-9C58B5F5C6ED}" name="AP" dataDxfId="56"/>
+    <tableColumn id="8" xr3:uid="{0E0FA7BD-E6EA-426B-B8B1-9665A67EE819}" name="PA" dataDxfId="55"/>
+    <tableColumn id="9" xr3:uid="{9ABF8262-0C59-4BAA-8D66-6D70743CECED}" name="TO" dataDxfId="54"/>
+    <tableColumn id="10" xr3:uid="{96D8ACAF-FFFE-4005-ADC1-94AA97CD6038}" name="NORDESTE" dataDxfId="53"/>
+    <tableColumn id="11" xr3:uid="{1FABF4C2-AC99-4575-B4A2-682FB02C27AB}" name="MA" dataDxfId="52"/>
+    <tableColumn id="12" xr3:uid="{6E7000A1-CF81-4A5C-AF79-B5A606493E58}" name="PI" dataDxfId="51"/>
+    <tableColumn id="13" xr3:uid="{5804C6F2-0132-4A60-8701-6454E76B39E1}" name="CE" dataDxfId="50"/>
+    <tableColumn id="14" xr3:uid="{FAC246D4-9925-4737-BA6E-C12890CC3492}" name="RN" dataDxfId="49"/>
+    <tableColumn id="15" xr3:uid="{70365A79-11D8-4822-868C-B390282D31AA}" name="PB" dataDxfId="48"/>
+    <tableColumn id="16" xr3:uid="{C5EA46D4-2A74-4A1B-8628-EDE27732EBC1}" name="PE" dataDxfId="47"/>
+    <tableColumn id="17" xr3:uid="{3AB16384-A9C1-4EAE-B1D3-B6980668DDFB}" name="AL" dataDxfId="46"/>
+    <tableColumn id="18" xr3:uid="{5550B480-640D-47F3-98E2-47360C39B350}" name="SE" dataDxfId="45"/>
+    <tableColumn id="19" xr3:uid="{AC7410A2-BEC3-4F36-9DE3-007ABEDAFE77}" name="BA" dataDxfId="44"/>
+    <tableColumn id="20" xr3:uid="{EF9CC834-4DE2-4F12-A01F-E188C35BB745}" name="CENTRO-OESTE" dataDxfId="43"/>
+    <tableColumn id="21" xr3:uid="{43361983-B660-4F10-8172-158B7FE088A3}" name="MT" dataDxfId="42"/>
+    <tableColumn id="22" xr3:uid="{1D87111A-4709-4B48-BC75-F06DA78D87CB}" name="MS" dataDxfId="41"/>
+    <tableColumn id="23" xr3:uid="{8C8B08DD-2483-4E25-AB6C-69DC01B3EB3D}" name="GO" dataDxfId="40"/>
+    <tableColumn id="24" xr3:uid="{9D3A4E55-E1CC-4509-9BBA-1BA1B5720931}" name="DF" dataDxfId="39"/>
+    <tableColumn id="25" xr3:uid="{64CEA2A0-9627-43CF-9192-24F44872CC96}" name="SUDESTE" dataDxfId="38"/>
+    <tableColumn id="26" xr3:uid="{4FBE3EC3-154E-4DF3-ABB6-B6DEFFC26271}" name="MG" dataDxfId="37"/>
+    <tableColumn id="27" xr3:uid="{B6B47D99-4133-4D01-BF64-2BBBE6D3BE49}" name="ES" dataDxfId="36"/>
+    <tableColumn id="28" xr3:uid="{7CC112A7-D0E8-4317-B401-EC4CD011155C}" name="RJ" dataDxfId="35"/>
+    <tableColumn id="29" xr3:uid="{14E6FF96-46F0-467D-A5A3-F1C831072AA9}" name="SP" dataDxfId="34"/>
+    <tableColumn id="30" xr3:uid="{932BDB91-3454-40CD-B097-52A8AA0A2F81}" name="SUL" dataDxfId="33"/>
+    <tableColumn id="31" xr3:uid="{AA858ED8-15B1-4985-9F57-E0EE2783C677}" name="PR" dataDxfId="32"/>
+    <tableColumn id="32" xr3:uid="{D302D227-008B-444D-87CF-C19499331330}" name="SC" dataDxfId="31"/>
+    <tableColumn id="33" xr3:uid="{65AB5642-25AB-4920-8029-D56BC42AB123}" name="RS" dataDxfId="30"/>
+    <tableColumn id="34" xr3:uid="{7666B84C-5946-494A-83CA-2B24D2CF0DC8}" name="NORTE-NORDESTE" dataDxfId="29"/>
+    <tableColumn id="35" xr3:uid="{633B8894-AE4A-45AC-B1C9-B4EAA702D9F9}" name="CENTRO-SUL" dataDxfId="28"/>
+    <tableColumn id="36" xr3:uid="{6BB08E62-BEF0-4192-83F6-2E12E9E586B8}" name="BRASIL" dataDxfId="27"/>
+    <tableColumn id="37" xr3:uid="{ECC44396-0C86-4DF0-B859-53097AD13988}" name="ANO" dataDxfId="26"/>
+    <tableColumn id="38" xr3:uid="{57AEF2DA-BFBE-4B5B-ABC0-477C4D3CA382}" name="MÊS" dataDxfId="25"/>
+    <tableColumn id="39" xr3:uid="{4AF1745A-E1C0-4A75-AFC1-E75F141DCCAA}" name="SAFRA" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1112,7 +1112,9 @@
     <tableColumn id="22" xr3:uid="{49B2C1E3-0396-4037-BB4B-32C18FDB6CC7}" name="CEVADA" dataDxfId="3"/>
     <tableColumn id="23" xr3:uid="{C10C34AB-D106-4FB2-B097-C90EF653E9E5}" name="TRIGO" dataDxfId="2"/>
     <tableColumn id="24" xr3:uid="{80045204-E6E2-42D6-9449-CCD3B9641988}" name="TRITICALE" dataDxfId="1"/>
-    <tableColumn id="25" xr3:uid="{0FB9C96B-75F4-4026-A109-A799A828C96B}" name="GERAL" dataDxfId="0"/>
+    <tableColumn id="25" xr3:uid="{0FB9C96B-75F4-4026-A109-A799A828C96B}" name="GERAL" dataDxfId="0">
+      <calculatedColumnFormula>SUM(B2,E2:F2,I2,M2:X2)</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="26" xr3:uid="{FA0650E0-02EE-433A-927B-8DCFAD627C43}" name="ANO"/>
     <tableColumn id="27" xr3:uid="{94C00EC6-AB2D-4D90-B787-2C1FF57B5832}" name="MÊS"/>
     <tableColumn id="28" xr3:uid="{57AFB38B-E07E-457A-9571-EB539326E109}" name="SAFRA"/>
@@ -1386,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AM25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:AJ25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4402,7 +4404,7 @@
   <dimension ref="A1:AB36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="B2" sqref="B2:Y36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5590,7 +5592,9 @@
       <c r="N14" s="1">
         <v>0</v>
       </c>
-      <c r="O14" s="1"/>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
       <c r="P14" s="1">
         <v>62.5</v>
       </c>
@@ -7537,7 +7541,7 @@
   <dimension ref="A1:AM26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="B2" sqref="B2:AJ25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13740,7 +13744,7 @@
   <dimension ref="A1:AM25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AM25"/>
+      <selection activeCell="B2" sqref="B2:AJ25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16616,109 +16620,144 @@
         <v>56</v>
       </c>
       <c r="B25" s="1">
-        <v>16052.400000000001</v>
+        <f>SUM(B2,B5:B6,B9,B13:B24)</f>
+        <v>15023.800000000001</v>
       </c>
       <c r="C25" s="1">
-        <v>638.59999999999991</v>
+        <f>SUM(C2,C5:C6,C9,C13:C24)</f>
+        <v>544.29999999999995</v>
       </c>
       <c r="D25" s="1">
-        <v>3425.1000000000004</v>
+        <f t="shared" ref="D25:AJ25" si="0">SUM(D2,D5:D6,D9,D13:D24)</f>
+        <v>3305.4</v>
       </c>
       <c r="E25" s="1">
-        <v>188.60000000000002</v>
+        <f t="shared" si="0"/>
+        <v>180.70000000000002</v>
       </c>
       <c r="F25" s="1">
-        <v>58</v>
+        <f t="shared" si="0"/>
+        <v>47.8</v>
       </c>
       <c r="G25" s="1">
-        <v>22.8</v>
+        <f t="shared" si="0"/>
+        <v>20.8</v>
       </c>
       <c r="H25" s="1">
-        <v>4481.3999999999996</v>
+        <f t="shared" si="0"/>
+        <v>4352.7</v>
       </c>
       <c r="I25" s="1">
-        <v>7237.9000000000005</v>
+        <f t="shared" si="0"/>
+        <v>6572.1</v>
       </c>
       <c r="J25" s="1">
-        <v>30947.700000000004</v>
+        <f t="shared" si="0"/>
+        <v>28276.400000000005</v>
       </c>
       <c r="K25" s="1">
-        <v>7529.1</v>
+        <f t="shared" si="0"/>
+        <v>7191.1</v>
       </c>
       <c r="L25" s="1">
-        <v>6397.7999999999993</v>
+        <f t="shared" si="0"/>
+        <v>6184.6999999999989</v>
       </c>
       <c r="M25" s="1">
-        <v>812.2</v>
+        <f t="shared" si="0"/>
+        <v>676.59999999999991</v>
       </c>
       <c r="N25" s="1">
-        <v>83.3</v>
+        <f t="shared" si="0"/>
+        <v>59.4</v>
       </c>
       <c r="O25" s="1">
-        <v>153.80000000000001</v>
+        <f t="shared" si="0"/>
+        <v>113.2</v>
       </c>
       <c r="P25" s="1">
-        <v>351.3</v>
+        <f t="shared" si="0"/>
+        <v>255.8</v>
       </c>
       <c r="Q25" s="1">
-        <v>140.9</v>
+        <f t="shared" si="0"/>
+        <v>116.9</v>
       </c>
       <c r="R25" s="1">
-        <v>1048.3</v>
+        <f t="shared" si="0"/>
+        <v>998.7</v>
       </c>
       <c r="S25" s="1">
-        <v>14431</v>
+        <f t="shared" si="0"/>
+        <v>12680</v>
       </c>
       <c r="T25" s="1">
-        <v>156476.39999999997</v>
+        <f t="shared" si="0"/>
+        <v>150096.99999999994</v>
       </c>
       <c r="U25" s="1">
-        <v>97256.799999999988</v>
+        <f t="shared" si="0"/>
+        <v>91632.4</v>
       </c>
       <c r="V25" s="1">
-        <v>25227.599999999999</v>
+        <f t="shared" si="0"/>
+        <v>25026.799999999996</v>
       </c>
       <c r="W25" s="1">
-        <v>33043.5</v>
+        <f t="shared" si="0"/>
+        <v>32528.1</v>
       </c>
       <c r="X25" s="1">
-        <v>948.5</v>
+        <f t="shared" si="0"/>
+        <v>909.69999999999993</v>
       </c>
       <c r="Y25" s="1">
-        <v>29564.800000000007</v>
+        <f t="shared" si="0"/>
+        <v>28695.500000000004</v>
       </c>
       <c r="Z25" s="1">
-        <v>18897.300000000003</v>
+        <f t="shared" si="0"/>
+        <v>18295.300000000003</v>
       </c>
       <c r="AA25" s="1">
-        <v>60.400000000000006</v>
+        <f t="shared" si="0"/>
+        <v>50.300000000000004</v>
       </c>
       <c r="AB25" s="1">
-        <v>11.1</v>
+        <f t="shared" si="0"/>
+        <v>9.1</v>
       </c>
       <c r="AC25" s="1">
-        <v>10596</v>
+        <f t="shared" si="0"/>
+        <v>10340.800000000001</v>
       </c>
       <c r="AD25" s="1">
-        <v>103151.49999999999</v>
+        <f t="shared" si="0"/>
+        <v>93197.299999999988</v>
       </c>
       <c r="AE25" s="1">
-        <v>46279.500000000007</v>
+        <f t="shared" si="0"/>
+        <v>45403.700000000004</v>
       </c>
       <c r="AF25" s="1">
-        <v>8609</v>
+        <f t="shared" si="0"/>
+        <v>7294.7</v>
       </c>
       <c r="AG25" s="1">
-        <v>48263</v>
+        <f t="shared" si="0"/>
+        <v>40498.9</v>
       </c>
       <c r="AH25" s="1">
-        <v>47000.100000000006</v>
+        <f t="shared" si="0"/>
+        <v>43300.200000000004</v>
       </c>
       <c r="AI25" s="1">
-        <v>289192.69999999995</v>
+        <f t="shared" si="0"/>
+        <v>271989.8</v>
       </c>
       <c r="AJ25" s="1">
-        <v>336192.8</v>
+        <f t="shared" si="0"/>
+        <v>315290</v>
       </c>
       <c r="AK25" s="2">
         <v>2022</v>
@@ -16742,8 +16781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37856A1E-82E7-45AE-A2B0-C510B7D63887}">
   <dimension ref="A1:AM36"/>
   <sheetViews>
-    <sheetView topLeftCell="J10" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:Y36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16938,7 +16977,8 @@
         <v>0</v>
       </c>
       <c r="Y2" s="1">
-        <v>16052.400000000001</v>
+        <f>SUM(B2,E2:F2,I2,M2:X2)</f>
+        <v>15023.800000000001</v>
       </c>
       <c r="Z2">
         <v>2022</v>
@@ -17024,7 +17064,8 @@
         <v>0</v>
       </c>
       <c r="Y3" s="1">
-        <v>638.59999999999991</v>
+        <f t="shared" ref="Y3:Y36" si="0">SUM(B3,E3:F3,I3,M3:X3)</f>
+        <v>544.29999999999995</v>
       </c>
       <c r="Z3">
         <v>2022</v>
@@ -17110,7 +17151,8 @@
         <v>0</v>
       </c>
       <c r="Y4" s="1">
-        <v>3425.1000000000004</v>
+        <f t="shared" si="0"/>
+        <v>3305.4</v>
       </c>
       <c r="Z4">
         <v>2022</v>
@@ -17196,7 +17238,8 @@
         <v>0</v>
       </c>
       <c r="Y5" s="1">
-        <v>188.60000000000002</v>
+        <f t="shared" si="0"/>
+        <v>180.70000000000002</v>
       </c>
       <c r="Z5">
         <v>2022</v>
@@ -17282,7 +17325,8 @@
         <v>0</v>
       </c>
       <c r="Y6" s="1">
-        <v>58</v>
+        <f t="shared" si="0"/>
+        <v>47.8</v>
       </c>
       <c r="Z6">
         <v>2022</v>
@@ -17368,7 +17412,8 @@
         <v>0</v>
       </c>
       <c r="Y7" s="1">
-        <v>22.8</v>
+        <f t="shared" si="0"/>
+        <v>20.8</v>
       </c>
       <c r="Z7">
         <v>2022</v>
@@ -17454,7 +17499,8 @@
         <v>0</v>
       </c>
       <c r="Y8" s="1">
-        <v>4481.3999999999996</v>
+        <f t="shared" si="0"/>
+        <v>4352.7</v>
       </c>
       <c r="Z8">
         <v>2022</v>
@@ -17540,7 +17586,8 @@
         <v>0</v>
       </c>
       <c r="Y9" s="1">
-        <v>7237.9000000000005</v>
+        <f t="shared" si="0"/>
+        <v>6572.1</v>
       </c>
       <c r="Z9">
         <v>2022</v>
@@ -17626,7 +17673,8 @@
         <v>0</v>
       </c>
       <c r="Y10" s="1">
-        <v>30947.700000000004</v>
+        <f t="shared" si="0"/>
+        <v>28276.400000000005</v>
       </c>
       <c r="Z10">
         <v>2022</v>
@@ -17712,7 +17760,8 @@
         <v>0</v>
       </c>
       <c r="Y11" s="1">
-        <v>7529.1</v>
+        <f t="shared" si="0"/>
+        <v>7191.1</v>
       </c>
       <c r="Z11">
         <v>2022</v>
@@ -17798,7 +17847,8 @@
         <v>0</v>
       </c>
       <c r="Y12" s="1">
-        <v>6397.7999999999993</v>
+        <f t="shared" si="0"/>
+        <v>6184.6999999999989</v>
       </c>
       <c r="Z12">
         <v>2022</v>
@@ -17884,7 +17934,8 @@
         <v>0</v>
       </c>
       <c r="Y13" s="1">
-        <v>812.2</v>
+        <f t="shared" si="0"/>
+        <v>676.59999999999991</v>
       </c>
       <c r="Z13">
         <v>2022</v>
@@ -17970,7 +18021,8 @@
         <v>0</v>
       </c>
       <c r="Y14" s="1">
-        <v>83.3</v>
+        <f t="shared" si="0"/>
+        <v>59.4</v>
       </c>
       <c r="Z14">
         <v>2022</v>
@@ -18056,7 +18108,8 @@
         <v>0</v>
       </c>
       <c r="Y15" s="1">
-        <v>153.80000000000001</v>
+        <f t="shared" si="0"/>
+        <v>113.2</v>
       </c>
       <c r="Z15">
         <v>2022</v>
@@ -18142,7 +18195,8 @@
         <v>0</v>
       </c>
       <c r="Y16" s="1">
-        <v>351.3</v>
+        <f t="shared" si="0"/>
+        <v>255.8</v>
       </c>
       <c r="Z16">
         <v>2022</v>
@@ -18228,7 +18282,8 @@
         <v>0</v>
       </c>
       <c r="Y17" s="1">
-        <v>140.9</v>
+        <f t="shared" si="0"/>
+        <v>116.9</v>
       </c>
       <c r="Z17">
         <v>2022</v>
@@ -18314,7 +18369,8 @@
         <v>0</v>
       </c>
       <c r="Y18" s="1">
-        <v>1048.3</v>
+        <f t="shared" si="0"/>
+        <v>998.7</v>
       </c>
       <c r="Z18">
         <v>2022</v>
@@ -18400,7 +18456,8 @@
         <v>0</v>
       </c>
       <c r="Y19" s="1">
-        <v>14431</v>
+        <f t="shared" si="0"/>
+        <v>12680</v>
       </c>
       <c r="Z19">
         <v>2022</v>
@@ -18486,7 +18543,8 @@
         <v>0</v>
       </c>
       <c r="Y20" s="1">
-        <v>156476.39999999997</v>
+        <f t="shared" si="0"/>
+        <v>150096.99999999994</v>
       </c>
       <c r="Z20">
         <v>2022</v>
@@ -18572,7 +18630,8 @@
         <v>0</v>
       </c>
       <c r="Y21" s="1">
-        <v>97256.799999999988</v>
+        <f t="shared" si="0"/>
+        <v>91632.4</v>
       </c>
       <c r="Z21">
         <v>2022</v>
@@ -18658,7 +18717,8 @@
         <v>0</v>
       </c>
       <c r="Y22" s="1">
-        <v>25227.599999999999</v>
+        <f t="shared" si="0"/>
+        <v>25026.799999999996</v>
       </c>
       <c r="Z22">
         <v>2022</v>
@@ -18744,7 +18804,8 @@
         <v>0</v>
       </c>
       <c r="Y23" s="1">
-        <v>33043.5</v>
+        <f t="shared" si="0"/>
+        <v>32528.1</v>
       </c>
       <c r="Z23">
         <v>2022</v>
@@ -18830,7 +18891,8 @@
         <v>0</v>
       </c>
       <c r="Y24" s="1">
-        <v>948.5</v>
+        <f t="shared" si="0"/>
+        <v>909.69999999999993</v>
       </c>
       <c r="Z24">
         <v>2022</v>
@@ -18916,7 +18978,8 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="Y25" s="1">
-        <v>29564.800000000007</v>
+        <f t="shared" si="0"/>
+        <v>28695.500000000004</v>
       </c>
       <c r="Z25">
         <v>2022</v>
@@ -19002,7 +19065,8 @@
         <v>0</v>
       </c>
       <c r="Y26" s="1">
-        <v>18897.300000000003</v>
+        <f t="shared" si="0"/>
+        <v>18295.300000000003</v>
       </c>
       <c r="Z26">
         <v>2022</v>
@@ -19099,7 +19163,8 @@
         <v>0</v>
       </c>
       <c r="Y27" s="1">
-        <v>60.400000000000006</v>
+        <f t="shared" si="0"/>
+        <v>50.300000000000004</v>
       </c>
       <c r="Z27">
         <v>2022</v>
@@ -19185,7 +19250,8 @@
         <v>0</v>
       </c>
       <c r="Y28" s="1">
-        <v>11.1</v>
+        <f t="shared" si="0"/>
+        <v>9.1</v>
       </c>
       <c r="Z28">
         <v>2022</v>
@@ -19271,7 +19337,8 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="Y29" s="1">
-        <v>10596</v>
+        <f t="shared" si="0"/>
+        <v>10340.800000000001</v>
       </c>
       <c r="Z29">
         <v>2022</v>
@@ -19357,7 +19424,8 @@
         <v>50.4</v>
       </c>
       <c r="Y30" s="1">
-        <v>103151.49999999999</v>
+        <f t="shared" si="0"/>
+        <v>93197.299999999988</v>
       </c>
       <c r="Z30">
         <v>2022</v>
@@ -19443,7 +19511,8 @@
         <v>32.799999999999997</v>
       </c>
       <c r="Y31" s="1">
-        <v>46279.500000000007</v>
+        <f t="shared" si="0"/>
+        <v>45403.700000000004</v>
       </c>
       <c r="Z31">
         <v>2022</v>
@@ -19529,7 +19598,8 @@
         <v>0</v>
       </c>
       <c r="Y32" s="1">
-        <v>8609</v>
+        <f t="shared" si="0"/>
+        <v>7294.7</v>
       </c>
       <c r="Z32">
         <v>2022</v>
@@ -19615,7 +19685,8 @@
         <v>17.600000000000001</v>
       </c>
       <c r="Y33" s="1">
-        <v>48263</v>
+        <f t="shared" si="0"/>
+        <v>40498.9</v>
       </c>
       <c r="Z33">
         <v>2022</v>
@@ -19701,7 +19772,8 @@
         <v>0</v>
       </c>
       <c r="Y34" s="1">
-        <v>47000.100000000006</v>
+        <f t="shared" si="0"/>
+        <v>43300.200000000004</v>
       </c>
       <c r="Z34">
         <v>2022</v>
@@ -19787,7 +19859,8 @@
         <v>60.099999999999994</v>
       </c>
       <c r="Y35" s="1">
-        <v>289192.69999999995</v>
+        <f t="shared" si="0"/>
+        <v>271989.8</v>
       </c>
       <c r="Z35">
         <v>2022</v>
@@ -19873,7 +19946,8 @@
         <v>60.099999999999994</v>
       </c>
       <c r="Y36" s="1">
-        <v>336192.8</v>
+        <f t="shared" si="0"/>
+        <v>315290</v>
       </c>
       <c r="Z36">
         <v>2022</v>

</xml_diff>